<commit_message>
#1 implemented a Sheet class to supercede Header and replace ix_list and contexts. Starting to implement a way to iterate through multiple tabs to create several tables.
</commit_message>
<xml_diff>
--- a/input_files/afcrs/example.xlsx
+++ b/input_files/afcrs/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/Process-XBRL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/afcrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E45118-5AB9-E149-8F0C-54D526BC4445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182CC011-725F-5741-B731-75B30869B0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31760" yWindow="-6600" windowWidth="28800" windowHeight="16020" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Governmental Activities</t>
   </si>
   <si>
-    <t>Business-Type Activites</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Total Assets</t>
+  </si>
+  <si>
+    <t>Business-Type Activities</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -605,16 +605,16 @@
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -623,7 +623,7 @@
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -631,16 +631,16 @@
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="C8" s="8">
         <v>13441679</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="8">
         <v>13441679</v>
@@ -648,16 +648,16 @@
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C9" s="9">
         <v>1133315</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="9">
         <v>1133315</v>
@@ -665,16 +665,16 @@
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="C10" s="9">
         <v>25257</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="9">
         <v>25257</v>
@@ -682,10 +682,10 @@
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="C11" s="9">
         <v>120893</v>
@@ -694,21 +694,21 @@
         <v>-120893</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="C12" s="9">
         <v>52578</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="9">
         <v>52578</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="C13" s="9">
         <v>14773722</v>
@@ -734,7 +734,7 @@
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -742,16 +742,16 @@
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="9">
         <v>3170453</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="9">
         <v>3170453</v>
@@ -759,16 +759,16 @@
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C16" s="9">
         <v>3311550</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="9">
         <v>3311550</v>
@@ -776,10 +776,10 @@
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="C17" s="9">
         <v>3133754</v>
@@ -793,10 +793,10 @@
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="C18" s="9">
         <v>25982451</v>
@@ -810,10 +810,10 @@
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C19" s="9">
         <v>35598208</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C20" s="10">
         <v>50371930</v>

</xml_diff>